<commit_message>
Conditional statements added to process lookup table drawio_shapes
</commit_message>
<xml_diff>
--- a/src/main/webapp/js/cktparser/drawio_circuitikz_v19082022.xlsx
+++ b/src/main/webapp/js/cktparser/drawio_circuitikz_v19082022.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yuriel\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yuriel\git\CJ1-drawio-circuitikz\src\main\webapp\js\cktparser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC99625-9D16-4CC1-9CCF-AC63F85F557C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948E3B45-D310-4FD0-9D1A-86A2C6DFB847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{ACCEF36F-F2B4-4F7F-83FE-D2DAA1238264}"/>
   </bookViews>
@@ -56,9 +56,6 @@
     <t>D type flip flop</t>
   </si>
   <si>
-    <t>mxgraph.electrical.logic_gates.inverter_2</t>
-  </si>
-  <si>
     <t>Inverter</t>
   </si>
   <si>
@@ -1382,16 +1379,19 @@
     <t>mxgraph.electrical.electro-mechanical.pushbutton;aspect=fixed;elSwitchState=on;</t>
   </si>
   <si>
-    <t>ellipse;value="M"</t>
-  </si>
-  <si>
-    <t>ellipse;value="A"</t>
-  </si>
-  <si>
-    <t>ellipse;value="V"</t>
-  </si>
-  <si>
     <t>mxgraph.electrical.signal_sources.source;elSignalType=dc3;elSourceType=dependent;</t>
+  </si>
+  <si>
+    <t>mxgraph.electrical.logic_gates.inverter_2;</t>
+  </si>
+  <si>
+    <t>ellipse;value="A";</t>
+  </si>
+  <si>
+    <t>ellipse;value="V";</t>
+  </si>
+  <si>
+    <t>ellipse;value="M";</t>
   </si>
 </sst>
 </file>
@@ -1753,9 +1753,9 @@
   <dimension ref="A1:H117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B54" sqref="B54"/>
+      <selection pane="bottomLeft" activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1767,22 +1767,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B1" t="s">
+        <v>330</v>
+      </c>
+      <c r="C1" t="s">
+        <v>333</v>
+      </c>
+      <c r="D1" t="s">
         <v>331</v>
-      </c>
-      <c r="C1" t="s">
-        <v>334</v>
-      </c>
-      <c r="D1" t="s">
-        <v>332</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -1790,19 +1790,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E2" t="s">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -1813,16 +1813,16 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -1833,16 +1833,16 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E4" t="s">
         <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -1850,19 +1850,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>448</v>
+      </c>
+      <c r="C5" t="s">
+        <v>338</v>
+      </c>
+      <c r="D5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
-        <v>339</v>
-      </c>
-      <c r="D5" t="s">
-        <v>136</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
-      </c>
       <c r="F5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -1870,19 +1870,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>339</v>
+      </c>
+      <c r="D6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
-        <v>340</v>
-      </c>
-      <c r="D6" t="s">
-        <v>136</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
       <c r="F6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -1890,19 +1890,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>340</v>
+      </c>
+      <c r="D7" t="s">
+        <v>135</v>
+      </c>
+      <c r="E7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" t="s">
-        <v>341</v>
-      </c>
-      <c r="D7" t="s">
-        <v>136</v>
-      </c>
-      <c r="E7" t="s">
-        <v>11</v>
-      </c>
       <c r="F7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -1910,19 +1910,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -1930,19 +1930,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -1950,19 +1950,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -1970,19 +1970,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1990,19 +1990,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>345</v>
+      </c>
+      <c r="D12" t="s">
+        <v>135</v>
+      </c>
+      <c r="E12" t="s">
         <v>21</v>
       </c>
-      <c r="C12" t="s">
-        <v>346</v>
-      </c>
-      <c r="D12" t="s">
-        <v>136</v>
-      </c>
-      <c r="E12" t="s">
-        <v>22</v>
-      </c>
       <c r="F12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -2010,19 +2010,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>346</v>
+      </c>
+      <c r="D13" t="s">
+        <v>135</v>
+      </c>
+      <c r="E13" t="s">
         <v>23</v>
       </c>
-      <c r="C13" t="s">
-        <v>347</v>
-      </c>
-      <c r="D13" t="s">
-        <v>136</v>
-      </c>
-      <c r="E13" t="s">
-        <v>24</v>
-      </c>
       <c r="F13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
@@ -2030,19 +2030,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -2050,19 +2050,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -2070,19 +2070,19 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
@@ -2090,19 +2090,19 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C17" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
@@ -2110,19 +2110,19 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" t="s">
+        <v>382</v>
+      </c>
+      <c r="D18" t="s">
+        <v>134</v>
+      </c>
+      <c r="E18" t="s">
         <v>33</v>
       </c>
-      <c r="C18" t="s">
-        <v>383</v>
-      </c>
-      <c r="D18" t="s">
-        <v>135</v>
-      </c>
-      <c r="E18" t="s">
-        <v>34</v>
-      </c>
       <c r="F18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
@@ -2130,22 +2130,22 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F19" t="s">
+        <v>50</v>
+      </c>
+      <c r="H19" t="s">
         <v>51</v>
-      </c>
-      <c r="H19" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
@@ -2153,22 +2153,22 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
@@ -2176,22 +2176,22 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C21" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F21" t="s">
+        <v>52</v>
+      </c>
+      <c r="H21" t="s">
         <v>53</v>
-      </c>
-      <c r="H21" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
@@ -2199,22 +2199,22 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D22" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F22" t="s">
+        <v>55</v>
+      </c>
+      <c r="H22" t="s">
         <v>56</v>
-      </c>
-      <c r="H22" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
@@ -2222,22 +2222,22 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" t="s">
+        <v>134</v>
+      </c>
+      <c r="E23" t="s">
         <v>43</v>
       </c>
-      <c r="C23" t="s">
-        <v>58</v>
-      </c>
-      <c r="D23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E23" t="s">
-        <v>44</v>
-      </c>
       <c r="F23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
@@ -2245,19 +2245,19 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" t="s">
+        <v>384</v>
+      </c>
+      <c r="D24" t="s">
+        <v>134</v>
+      </c>
+      <c r="E24" t="s">
         <v>45</v>
       </c>
-      <c r="C24" t="s">
-        <v>385</v>
-      </c>
-      <c r="D24" t="s">
-        <v>135</v>
-      </c>
-      <c r="E24" t="s">
-        <v>46</v>
-      </c>
       <c r="F24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
@@ -2265,22 +2265,22 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C25" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D25" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F25" t="s">
+        <v>58</v>
+      </c>
+      <c r="H25" t="s">
         <v>59</v>
-      </c>
-      <c r="H25" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
@@ -2288,22 +2288,22 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" t="s">
+        <v>386</v>
+      </c>
+      <c r="D26" t="s">
+        <v>134</v>
+      </c>
+      <c r="E26" t="s">
         <v>49</v>
       </c>
-      <c r="C26" t="s">
-        <v>387</v>
-      </c>
-      <c r="D26" t="s">
-        <v>135</v>
-      </c>
-      <c r="E26" t="s">
-        <v>50</v>
-      </c>
       <c r="F26" t="s">
+        <v>61</v>
+      </c>
+      <c r="H26" t="s">
         <v>62</v>
-      </c>
-      <c r="H26" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
@@ -2311,19 +2311,19 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C27" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F27" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
@@ -2331,19 +2331,19 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C28" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D28" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F28" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
@@ -2351,19 +2351,19 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C29" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F29" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
@@ -2371,19 +2371,19 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C30" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E30" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F30" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
@@ -2391,19 +2391,19 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C31" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
@@ -2411,19 +2411,19 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C32" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D32" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F32" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
@@ -2431,19 +2431,19 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C33" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F33" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
@@ -2451,19 +2451,19 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C34" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D34" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E34" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F34" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
@@ -2471,19 +2471,19 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
+        <v>92</v>
+      </c>
+      <c r="C35" t="s">
+        <v>441</v>
+      </c>
+      <c r="D35" t="s">
+        <v>135</v>
+      </c>
+      <c r="E35" t="s">
         <v>93</v>
       </c>
-      <c r="C35" t="s">
-        <v>442</v>
-      </c>
-      <c r="D35" t="s">
-        <v>136</v>
-      </c>
-      <c r="E35" t="s">
-        <v>94</v>
-      </c>
       <c r="F35" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
@@ -2491,19 +2491,19 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
+        <v>94</v>
+      </c>
+      <c r="C36" t="s">
+        <v>440</v>
+      </c>
+      <c r="D36" t="s">
+        <v>135</v>
+      </c>
+      <c r="E36" t="s">
         <v>95</v>
       </c>
-      <c r="C36" t="s">
-        <v>441</v>
-      </c>
-      <c r="D36" t="s">
-        <v>136</v>
-      </c>
-      <c r="E36" t="s">
-        <v>96</v>
-      </c>
       <c r="F36" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
@@ -2511,19 +2511,19 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C37" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D37" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E37" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F37" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
@@ -2531,19 +2531,19 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C38" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D38" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E38" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F38" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
@@ -2551,19 +2551,19 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C39" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D39" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E39" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F39" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
@@ -2571,19 +2571,19 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C40" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D40" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E40" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F40" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
@@ -2591,19 +2591,19 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C41" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D41" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E41" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F41" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
@@ -2611,19 +2611,19 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C42" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D42" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E42" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F42" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
@@ -2631,19 +2631,19 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C43" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D43" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E43" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F43" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
@@ -2651,19 +2651,19 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C44" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D44" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E44" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F44" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
@@ -2671,19 +2671,19 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C45" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D45" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E45" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F45" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
@@ -2691,19 +2691,19 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C46" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D46" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E46" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F46" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
@@ -2711,19 +2711,19 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C47" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D47" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E47" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F47" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
@@ -2731,19 +2731,19 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C48" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D48" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E48" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F48" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.35">
@@ -2751,19 +2751,19 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C49" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D49" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E49" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F49" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
@@ -2771,19 +2771,19 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C50" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D50" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E50" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F50" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.35">
@@ -2791,19 +2791,19 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C51" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D51" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E51" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F51" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
@@ -2811,19 +2811,19 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C52" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D52" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E52" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F52" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.35">
@@ -2831,19 +2831,19 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="C53" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D53" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E53" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F53" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
@@ -2851,19 +2851,19 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C54" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D54" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E54" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F54" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.35">
@@ -2871,19 +2871,19 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C55" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D55" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E55" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F55" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.35">
@@ -2891,19 +2891,19 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C56" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D56" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E56" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F56" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.35">
@@ -2911,19 +2911,19 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C57" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D57" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E57" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F57" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
@@ -2931,19 +2931,19 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C58" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D58" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E58" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F58" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.35">
@@ -2951,19 +2951,19 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C59" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D59" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E59" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F59" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.35">
@@ -2971,19 +2971,19 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C60" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D60" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E60" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F60" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.35">
@@ -2991,19 +2991,19 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C61" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D61" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E61" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F61" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.35">
@@ -3011,19 +3011,19 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C62" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D62" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E62" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F62" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.35">
@@ -3031,19 +3031,19 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C63" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D63" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E63" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F63" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.35">
@@ -3051,19 +3051,19 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C64" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D64" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E64" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F64" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.35">
@@ -3071,19 +3071,19 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C65" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D65" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E65" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F65" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.35">
@@ -3091,19 +3091,19 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C66" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D66" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E66" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F66" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.35">
@@ -3111,19 +3111,19 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C67" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D67" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E67" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F67" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.35">
@@ -3131,19 +3131,19 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C68" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D68" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E68" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F68" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.35">
@@ -3151,19 +3151,19 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C69" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D69" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E69" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F69" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.35">
@@ -3171,19 +3171,19 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C70" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D70" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E70" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F70" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.35">
@@ -3191,19 +3191,19 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C71" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D71" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E71" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F71" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.35">
@@ -3211,19 +3211,19 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C72" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D72" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E72" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F72" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.35">
@@ -3231,19 +3231,19 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C73" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D73" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E73" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F73" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.35">
@@ -3254,16 +3254,16 @@
         <v>449</v>
       </c>
       <c r="C74" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D74" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E74" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F74" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.35">
@@ -3271,19 +3271,19 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C75" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D75" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E75" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F75" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.35">
@@ -3294,16 +3294,16 @@
         <v>450</v>
       </c>
       <c r="C76" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D76" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E76" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F76" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.35">
@@ -3311,19 +3311,19 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
+        <v>217</v>
+      </c>
+      <c r="C77" t="s">
+        <v>416</v>
+      </c>
+      <c r="D77" t="s">
+        <v>134</v>
+      </c>
+      <c r="E77" t="s">
+        <v>216</v>
+      </c>
+      <c r="F77" t="s">
         <v>218</v>
-      </c>
-      <c r="C77" t="s">
-        <v>417</v>
-      </c>
-      <c r="D77" t="s">
-        <v>135</v>
-      </c>
-      <c r="E77" t="s">
-        <v>217</v>
-      </c>
-      <c r="F77" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.35">
@@ -3331,19 +3331,19 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
+        <v>220</v>
+      </c>
+      <c r="C78" t="s">
+        <v>417</v>
+      </c>
+      <c r="D78" t="s">
+        <v>134</v>
+      </c>
+      <c r="E78" t="s">
+        <v>219</v>
+      </c>
+      <c r="F78" t="s">
         <v>221</v>
-      </c>
-      <c r="C78" t="s">
-        <v>418</v>
-      </c>
-      <c r="D78" t="s">
-        <v>135</v>
-      </c>
-      <c r="E78" t="s">
-        <v>220</v>
-      </c>
-      <c r="F78" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.35">
@@ -3351,19 +3351,19 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C79" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D79" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E79" t="s">
+        <v>214</v>
+      </c>
+      <c r="F79" t="s">
         <v>215</v>
-      </c>
-      <c r="F79" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.35">
@@ -3371,19 +3371,19 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C80" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D80" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E80" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F80" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.35">
@@ -3391,19 +3391,19 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C81" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D81" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E81" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F81" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.35">
@@ -3411,19 +3411,19 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C82" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D82" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E82" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F82" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.35">
@@ -3431,19 +3431,19 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C83" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D83" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E83" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F83" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.35">
@@ -3451,19 +3451,19 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C84" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D84" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E84" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F84" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.35">
@@ -3471,19 +3471,19 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C85" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D85" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E85" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F85" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.35">
@@ -3491,19 +3491,19 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C86" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D86" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E86" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F86" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.35">
@@ -3511,19 +3511,19 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C87" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D87" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E87" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F87" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.35">
@@ -3531,19 +3531,19 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C88" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D88" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E88" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F88" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.35">
@@ -3551,19 +3551,19 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C89" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D89" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E89" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F89" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.35">
@@ -3571,19 +3571,19 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
+        <v>253</v>
+      </c>
+      <c r="C90" t="s">
+        <v>370</v>
+      </c>
+      <c r="D90" t="s">
+        <v>135</v>
+      </c>
+      <c r="E90" t="s">
+        <v>252</v>
+      </c>
+      <c r="F90" t="s">
         <v>254</v>
-      </c>
-      <c r="C90" t="s">
-        <v>371</v>
-      </c>
-      <c r="D90" t="s">
-        <v>136</v>
-      </c>
-      <c r="E90" t="s">
-        <v>253</v>
-      </c>
-      <c r="F90" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.35">
@@ -3591,19 +3591,19 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C91" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D91" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E91" t="s">
+        <v>255</v>
+      </c>
+      <c r="F91" t="s">
         <v>256</v>
-      </c>
-      <c r="F91" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.35">
@@ -3611,19 +3611,19 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C92" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D92" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E92" t="s">
+        <v>257</v>
+      </c>
+      <c r="F92" t="s">
         <v>258</v>
-      </c>
-      <c r="F92" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.35">
@@ -3631,19 +3631,19 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C93" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D93" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E93" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F93" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.35">
@@ -3651,19 +3651,19 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C94" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D94" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E94" t="s">
+        <v>260</v>
+      </c>
+      <c r="F94" t="s">
         <v>261</v>
-      </c>
-      <c r="F94" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.35">
@@ -3671,19 +3671,19 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
+        <v>264</v>
+      </c>
+      <c r="C95" t="s">
+        <v>371</v>
+      </c>
+      <c r="D95" t="s">
+        <v>135</v>
+      </c>
+      <c r="E95" t="s">
+        <v>263</v>
+      </c>
+      <c r="F95" t="s">
         <v>265</v>
-      </c>
-      <c r="C95" t="s">
-        <v>372</v>
-      </c>
-      <c r="D95" t="s">
-        <v>136</v>
-      </c>
-      <c r="E95" t="s">
-        <v>264</v>
-      </c>
-      <c r="F95" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.35">
@@ -3691,19 +3691,19 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C96" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D96" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E96" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F96" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.35">
@@ -3711,19 +3711,19 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
       <c r="C97" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D97" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E97" t="s">
+        <v>267</v>
+      </c>
+      <c r="F97" t="s">
         <v>268</v>
-      </c>
-      <c r="F97" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.35">
@@ -3731,19 +3731,19 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C98" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D98" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E98" t="s">
+        <v>269</v>
+      </c>
+      <c r="F98" t="s">
         <v>270</v>
-      </c>
-      <c r="F98" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.35">
@@ -3751,19 +3751,19 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C99" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D99" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E99" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F99" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.35">
@@ -3771,19 +3771,19 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
+        <v>276</v>
+      </c>
+      <c r="C100" t="s">
+        <v>428</v>
+      </c>
+      <c r="D100" t="s">
+        <v>134</v>
+      </c>
+      <c r="E100" t="s">
+        <v>275</v>
+      </c>
+      <c r="F100" t="s">
         <v>277</v>
-      </c>
-      <c r="C100" t="s">
-        <v>429</v>
-      </c>
-      <c r="D100" t="s">
-        <v>135</v>
-      </c>
-      <c r="E100" t="s">
-        <v>276</v>
-      </c>
-      <c r="F100" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.35">
@@ -3791,19 +3791,19 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
+        <v>279</v>
+      </c>
+      <c r="C101" t="s">
+        <v>429</v>
+      </c>
+      <c r="D101" t="s">
+        <v>134</v>
+      </c>
+      <c r="E101" t="s">
         <v>280</v>
       </c>
-      <c r="C101" t="s">
-        <v>430</v>
-      </c>
-      <c r="D101" t="s">
-        <v>135</v>
-      </c>
-      <c r="E101" t="s">
-        <v>281</v>
-      </c>
       <c r="F101" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.35">
@@ -3811,19 +3811,19 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C102" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D102" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E102" t="s">
+        <v>281</v>
+      </c>
+      <c r="F102" t="s">
         <v>282</v>
-      </c>
-      <c r="F102" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.35">
@@ -3831,19 +3831,19 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C103" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D103" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E103" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F103" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.35">
@@ -3851,19 +3851,19 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
+        <v>288</v>
+      </c>
+      <c r="C104" t="s">
+        <v>432</v>
+      </c>
+      <c r="D104" t="s">
+        <v>134</v>
+      </c>
+      <c r="E104" t="s">
+        <v>287</v>
+      </c>
+      <c r="F104" t="s">
         <v>289</v>
-      </c>
-      <c r="C104" t="s">
-        <v>433</v>
-      </c>
-      <c r="D104" t="s">
-        <v>135</v>
-      </c>
-      <c r="E104" t="s">
-        <v>288</v>
-      </c>
-      <c r="F104" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.35">
@@ -3871,19 +3871,19 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C105" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D105" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E105" t="s">
+        <v>290</v>
+      </c>
+      <c r="F105" t="s">
         <v>291</v>
-      </c>
-      <c r="F105" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.35">
@@ -3891,19 +3891,19 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
+        <v>293</v>
+      </c>
+      <c r="C106" t="s">
+        <v>374</v>
+      </c>
+      <c r="D106" t="s">
+        <v>135</v>
+      </c>
+      <c r="E106" t="s">
         <v>294</v>
       </c>
-      <c r="C106" t="s">
-        <v>375</v>
-      </c>
-      <c r="D106" t="s">
-        <v>136</v>
-      </c>
-      <c r="E106" t="s">
-        <v>295</v>
-      </c>
       <c r="F106" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.35">
@@ -3911,19 +3911,19 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C107" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D107" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E107" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F107" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.35">
@@ -3931,19 +3931,19 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C108" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D108" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E108" t="s">
+        <v>299</v>
+      </c>
+      <c r="F108" t="s">
         <v>300</v>
-      </c>
-      <c r="F108" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.35">
@@ -3951,19 +3951,19 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
+        <v>302</v>
+      </c>
+      <c r="C109" t="s">
+        <v>377</v>
+      </c>
+      <c r="D109" t="s">
+        <v>135</v>
+      </c>
+      <c r="E109" t="s">
+        <v>299</v>
+      </c>
+      <c r="F109" t="s">
         <v>303</v>
-      </c>
-      <c r="C109" t="s">
-        <v>378</v>
-      </c>
-      <c r="D109" t="s">
-        <v>136</v>
-      </c>
-      <c r="E109" t="s">
-        <v>300</v>
-      </c>
-      <c r="F109" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.35">
@@ -3971,19 +3971,19 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
+        <v>305</v>
+      </c>
+      <c r="C110" t="s">
+        <v>378</v>
+      </c>
+      <c r="D110" t="s">
+        <v>135</v>
+      </c>
+      <c r="E110" t="s">
         <v>306</v>
       </c>
-      <c r="C110" t="s">
-        <v>379</v>
-      </c>
-      <c r="D110" t="s">
-        <v>136</v>
-      </c>
-      <c r="E110" t="s">
-        <v>307</v>
-      </c>
       <c r="F110" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.35">
@@ -3991,19 +3991,19 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
+        <v>307</v>
+      </c>
+      <c r="C111" t="s">
+        <v>379</v>
+      </c>
+      <c r="D111" t="s">
+        <v>135</v>
+      </c>
+      <c r="E111" t="s">
+        <v>306</v>
+      </c>
+      <c r="F111" t="s">
         <v>308</v>
-      </c>
-      <c r="C111" t="s">
-        <v>380</v>
-      </c>
-      <c r="D111" t="s">
-        <v>136</v>
-      </c>
-      <c r="E111" t="s">
-        <v>307</v>
-      </c>
-      <c r="F111" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.35">
@@ -4011,19 +4011,19 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
+        <v>310</v>
+      </c>
+      <c r="C112" t="s">
+        <v>434</v>
+      </c>
+      <c r="D112" t="s">
+        <v>134</v>
+      </c>
+      <c r="E112" t="s">
+        <v>309</v>
+      </c>
+      <c r="F112" t="s">
         <v>311</v>
-      </c>
-      <c r="C112" t="s">
-        <v>435</v>
-      </c>
-      <c r="D112" t="s">
-        <v>135</v>
-      </c>
-      <c r="E112" t="s">
-        <v>310</v>
-      </c>
-      <c r="F112" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.35">
@@ -4031,19 +4031,19 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
+        <v>312</v>
+      </c>
+      <c r="C113" t="s">
+        <v>435</v>
+      </c>
+      <c r="D113" t="s">
+        <v>134</v>
+      </c>
+      <c r="E113" t="s">
         <v>313</v>
       </c>
-      <c r="C113" t="s">
-        <v>436</v>
-      </c>
-      <c r="D113" t="s">
-        <v>135</v>
-      </c>
-      <c r="E113" t="s">
+      <c r="F113" t="s">
         <v>314</v>
-      </c>
-      <c r="F113" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.35">
@@ -4051,19 +4051,19 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
+        <v>316</v>
+      </c>
+      <c r="C114" t="s">
+        <v>436</v>
+      </c>
+      <c r="D114" t="s">
+        <v>134</v>
+      </c>
+      <c r="E114" t="s">
+        <v>315</v>
+      </c>
+      <c r="F114" t="s">
         <v>317</v>
-      </c>
-      <c r="C114" t="s">
-        <v>437</v>
-      </c>
-      <c r="D114" t="s">
-        <v>135</v>
-      </c>
-      <c r="E114" t="s">
-        <v>316</v>
-      </c>
-      <c r="F114" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.35">
@@ -4071,19 +4071,19 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C115" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D115" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E115" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F115" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.35">
@@ -4091,19 +4091,19 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
+        <v>321</v>
+      </c>
+      <c r="C116" t="s">
+        <v>381</v>
+      </c>
+      <c r="D116" t="s">
+        <v>135</v>
+      </c>
+      <c r="E116" t="s">
         <v>322</v>
       </c>
-      <c r="C116" t="s">
-        <v>382</v>
-      </c>
-      <c r="D116" t="s">
-        <v>136</v>
-      </c>
-      <c r="E116" t="s">
+      <c r="F116" t="s">
         <v>323</v>
-      </c>
-      <c r="F116" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="117" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -4111,23 +4111,24 @@
         <v>116</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F117" xr:uid="{A398772A-703D-48FD-983F-987E309B1154}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Latest version, paths work but nodes don't connect with lines
</commit_message>
<xml_diff>
--- a/src/main/webapp/js/cktparser/drawio_circuitikz_v19082022.xlsx
+++ b/src/main/webapp/js/cktparser/drawio_circuitikz_v19082022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yuriel\git\CJ1-drawio-circuitikz\src\main\webapp\js\cktparser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948E3B45-D310-4FD0-9D1A-86A2C6DFB847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE8E07E-F562-4257-9899-53576E312154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{ACCEF36F-F2B4-4F7F-83FE-D2DAA1238264}"/>
   </bookViews>
@@ -1040,9 +1040,6 @@
     <t>CircuitikzShape</t>
   </si>
   <si>
-    <t>Number</t>
-  </si>
-  <si>
     <t>node[ieeestd and port]{}</t>
   </si>
   <si>
@@ -1085,12 +1082,6 @@
     <t>node[ieeestd xnor port]{}</t>
   </si>
   <si>
-    <t>node[dipchip]{}</t>
-  </si>
-  <si>
-    <t>node[qfpchip]{}</t>
-  </si>
-  <si>
     <t>node[transformer]{}</t>
   </si>
   <si>
@@ -1392,6 +1383,15 @@
   </si>
   <si>
     <t>ellipse;value="M";</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>node[qfpchip, num pin=32]{}</t>
+  </si>
+  <si>
+    <t>node[dipchip, num pin=20]{}</t>
   </si>
 </sst>
 </file>
@@ -1407,7 +1407,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1417,6 +1417,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1433,9 +1439,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1753,13 +1760,14 @@
   <dimension ref="A1:H117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C88" sqref="C88"/>
+      <selection pane="bottomLeft" activeCell="B118" sqref="B118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46.6328125" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
     <col min="5" max="5" width="26.81640625" customWidth="1"/>
@@ -1767,7 +1775,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>334</v>
+        <v>449</v>
       </c>
       <c r="B1" t="s">
         <v>330</v>
@@ -1793,7 +1801,7 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D2" t="s">
         <v>135</v>
@@ -1813,7 +1821,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D3" t="s">
         <v>135</v>
@@ -1833,7 +1841,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D4" t="s">
         <v>135</v>
@@ -1850,10 +1858,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="C5" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D5" t="s">
         <v>135</v>
@@ -1873,7 +1881,7 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D6" t="s">
         <v>135</v>
@@ -1893,7 +1901,7 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D7" t="s">
         <v>135</v>
@@ -1913,7 +1921,7 @@
         <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D8" t="s">
         <v>135</v>
@@ -1933,7 +1941,7 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D9" t="s">
         <v>135</v>
@@ -1953,7 +1961,7 @@
         <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D10" t="s">
         <v>135</v>
@@ -1973,7 +1981,7 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D11" t="s">
         <v>135</v>
@@ -1993,7 +2001,7 @@
         <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D12" t="s">
         <v>135</v>
@@ -2013,7 +2021,7 @@
         <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D13" t="s">
         <v>135</v>
@@ -2033,7 +2041,7 @@
         <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D14" t="s">
         <v>135</v>
@@ -2053,7 +2061,7 @@
         <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D15" t="s">
         <v>135</v>
@@ -2065,43 +2073,43 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16">
+    <row r="16" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C16" t="s">
-        <v>349</v>
-      </c>
-      <c r="D16" t="s">
-        <v>135</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="C16" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17">
+    <row r="17" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C17" t="s">
-        <v>350</v>
-      </c>
-      <c r="D17" t="s">
-        <v>135</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="C17" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="2" t="s">
         <v>78</v>
       </c>
     </row>
@@ -2113,7 +2121,7 @@
         <v>32</v>
       </c>
       <c r="C18" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="D18" t="s">
         <v>134</v>
@@ -2156,7 +2164,7 @@
         <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D20" t="s">
         <v>134</v>
@@ -2179,7 +2187,7 @@
         <v>37</v>
       </c>
       <c r="C21" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D21" t="s">
         <v>134</v>
@@ -2248,7 +2256,7 @@
         <v>44</v>
       </c>
       <c r="C24" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="D24" t="s">
         <v>134</v>
@@ -2268,7 +2276,7 @@
         <v>47</v>
       </c>
       <c r="C25" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D25" t="s">
         <v>134</v>
@@ -2291,7 +2299,7 @@
         <v>48</v>
       </c>
       <c r="C26" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="D26" t="s">
         <v>134</v>
@@ -2314,7 +2322,7 @@
         <v>80</v>
       </c>
       <c r="C27" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="D27" t="s">
         <v>134</v>
@@ -2334,7 +2342,7 @@
         <v>81</v>
       </c>
       <c r="C28" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D28" t="s">
         <v>134</v>
@@ -2354,7 +2362,7 @@
         <v>82</v>
       </c>
       <c r="C29" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="D29" t="s">
         <v>134</v>
@@ -2374,7 +2382,7 @@
         <v>83</v>
       </c>
       <c r="C30" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="D30" t="s">
         <v>134</v>
@@ -2394,7 +2402,7 @@
         <v>86</v>
       </c>
       <c r="C31" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="D31" t="s">
         <v>134</v>
@@ -2414,7 +2422,7 @@
         <v>87</v>
       </c>
       <c r="C32" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="D32" t="s">
         <v>134</v>
@@ -2434,7 +2442,7 @@
         <v>88</v>
       </c>
       <c r="C33" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D33" t="s">
         <v>134</v>
@@ -2454,7 +2462,7 @@
         <v>89</v>
       </c>
       <c r="C34" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D34" t="s">
         <v>134</v>
@@ -2474,7 +2482,7 @@
         <v>92</v>
       </c>
       <c r="C35" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="D35" t="s">
         <v>135</v>
@@ -2494,7 +2502,7 @@
         <v>94</v>
       </c>
       <c r="C36" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="D36" t="s">
         <v>135</v>
@@ -2514,7 +2522,7 @@
         <v>103</v>
       </c>
       <c r="C37" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D37" t="s">
         <v>135</v>
@@ -2534,7 +2542,7 @@
         <v>105</v>
       </c>
       <c r="C38" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="D38" t="s">
         <v>134</v>
@@ -2554,7 +2562,7 @@
         <v>108</v>
       </c>
       <c r="C39" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D39" t="s">
         <v>134</v>
@@ -2574,7 +2582,7 @@
         <v>118</v>
       </c>
       <c r="C40" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="D40" t="s">
         <v>134</v>
@@ -2594,7 +2602,7 @@
         <v>119</v>
       </c>
       <c r="C41" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="D41" t="s">
         <v>134</v>
@@ -2614,7 +2622,7 @@
         <v>120</v>
       </c>
       <c r="C42" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="D42" t="s">
         <v>134</v>
@@ -2634,7 +2642,7 @@
         <v>121</v>
       </c>
       <c r="C43" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="D43" t="s">
         <v>134</v>
@@ -2654,7 +2662,7 @@
         <v>122</v>
       </c>
       <c r="C44" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="D44" t="s">
         <v>134</v>
@@ -2674,7 +2682,7 @@
         <v>123</v>
       </c>
       <c r="C45" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="D45" t="s">
         <v>134</v>
@@ -2694,7 +2702,7 @@
         <v>124</v>
       </c>
       <c r="C46" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="D46" t="s">
         <v>134</v>
@@ -2714,7 +2722,7 @@
         <v>125</v>
       </c>
       <c r="C47" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="D47" t="s">
         <v>134</v>
@@ -2734,7 +2742,7 @@
         <v>142</v>
       </c>
       <c r="C48" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="D48" t="s">
         <v>134</v>
@@ -2754,7 +2762,7 @@
         <v>145</v>
       </c>
       <c r="C49" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="D49" t="s">
         <v>134</v>
@@ -2774,7 +2782,7 @@
         <v>149</v>
       </c>
       <c r="C50" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D50" t="s">
         <v>134</v>
@@ -2794,7 +2802,7 @@
         <v>148</v>
       </c>
       <c r="C51" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="D51" t="s">
         <v>134</v>
@@ -2814,7 +2822,7 @@
         <v>150</v>
       </c>
       <c r="C52" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="D52" t="s">
         <v>134</v>
@@ -2831,10 +2839,10 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="C53" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D53" t="s">
         <v>134</v>
@@ -2854,7 +2862,7 @@
         <v>153</v>
       </c>
       <c r="C54" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="D54" t="s">
         <v>134</v>
@@ -2874,7 +2882,7 @@
         <v>109</v>
       </c>
       <c r="C55" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="D55" t="s">
         <v>134</v>
@@ -2894,7 +2902,7 @@
         <v>146</v>
       </c>
       <c r="C56" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="D56" t="s">
         <v>134</v>
@@ -2914,7 +2922,7 @@
         <v>147</v>
       </c>
       <c r="C57" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D57" t="s">
         <v>134</v>
@@ -2934,7 +2942,7 @@
         <v>152</v>
       </c>
       <c r="C58" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="D58" t="s">
         <v>134</v>
@@ -2954,7 +2962,7 @@
         <v>151</v>
       </c>
       <c r="C59" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="D59" t="s">
         <v>134</v>
@@ -2974,7 +2982,7 @@
         <v>178</v>
       </c>
       <c r="C60" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D60" t="s">
         <v>135</v>
@@ -2994,7 +3002,7 @@
         <v>179</v>
       </c>
       <c r="C61" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D61" t="s">
         <v>135</v>
@@ -3014,7 +3022,7 @@
         <v>180</v>
       </c>
       <c r="C62" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="D62" t="s">
         <v>135</v>
@@ -3034,7 +3042,7 @@
         <v>181</v>
       </c>
       <c r="C63" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="D63" t="s">
         <v>135</v>
@@ -3054,7 +3062,7 @@
         <v>182</v>
       </c>
       <c r="C64" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="D64" t="s">
         <v>135</v>
@@ -3074,7 +3082,7 @@
         <v>183</v>
       </c>
       <c r="C65" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="D65" t="s">
         <v>135</v>
@@ -3094,7 +3102,7 @@
         <v>184</v>
       </c>
       <c r="C66" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="D66" t="s">
         <v>135</v>
@@ -3114,7 +3122,7 @@
         <v>185</v>
       </c>
       <c r="C67" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="D67" t="s">
         <v>135</v>
@@ -3134,7 +3142,7 @@
         <v>186</v>
       </c>
       <c r="C68" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D68" t="s">
         <v>135</v>
@@ -3154,7 +3162,7 @@
         <v>187</v>
       </c>
       <c r="C69" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="D69" t="s">
         <v>135</v>
@@ -3174,7 +3182,7 @@
         <v>188</v>
       </c>
       <c r="C70" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="D70" t="s">
         <v>135</v>
@@ -3194,7 +3202,7 @@
         <v>189</v>
       </c>
       <c r="C71" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="D71" t="s">
         <v>135</v>
@@ -3214,7 +3222,7 @@
         <v>190</v>
       </c>
       <c r="C72" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="D72" t="s">
         <v>135</v>
@@ -3234,7 +3242,7 @@
         <v>191</v>
       </c>
       <c r="C73" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="D73" t="s">
         <v>135</v>
@@ -3251,10 +3259,10 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="C74" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="D74" t="s">
         <v>134</v>
@@ -3274,7 +3282,7 @@
         <v>205</v>
       </c>
       <c r="C75" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="D75" t="s">
         <v>134</v>
@@ -3291,10 +3299,10 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="C76" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="D76" t="s">
         <v>134</v>
@@ -3314,7 +3322,7 @@
         <v>217</v>
       </c>
       <c r="C77" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="D77" t="s">
         <v>134</v>
@@ -3334,7 +3342,7 @@
         <v>220</v>
       </c>
       <c r="C78" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="D78" t="s">
         <v>134</v>
@@ -3354,7 +3362,7 @@
         <v>222</v>
       </c>
       <c r="C79" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D79" t="s">
         <v>134</v>
@@ -3374,7 +3382,7 @@
         <v>229</v>
       </c>
       <c r="C80" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="D80" t="s">
         <v>135</v>
@@ -3414,7 +3422,7 @@
         <v>231</v>
       </c>
       <c r="C82" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="D82" t="s">
         <v>134</v>
@@ -3434,7 +3442,7 @@
         <v>232</v>
       </c>
       <c r="C83" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="D83" t="s">
         <v>134</v>
@@ -3454,7 +3462,7 @@
         <v>233</v>
       </c>
       <c r="C84" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="D84" t="s">
         <v>134</v>
@@ -3474,7 +3482,7 @@
         <v>234</v>
       </c>
       <c r="C85" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="D85" t="s">
         <v>134</v>
@@ -3494,7 +3502,7 @@
         <v>244</v>
       </c>
       <c r="C86" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="D86" t="s">
         <v>135</v>
@@ -3514,7 +3522,7 @@
         <v>245</v>
       </c>
       <c r="C87" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="D87" t="s">
         <v>135</v>
@@ -3534,7 +3542,7 @@
         <v>246</v>
       </c>
       <c r="C88" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="D88" t="s">
         <v>135</v>
@@ -3554,7 +3562,7 @@
         <v>247</v>
       </c>
       <c r="C89" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="D89" t="s">
         <v>135</v>
@@ -3574,7 +3582,7 @@
         <v>253</v>
       </c>
       <c r="C90" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="D90" t="s">
         <v>135</v>
@@ -3591,10 +3599,10 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="C91" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="D91" t="s">
         <v>134</v>
@@ -3611,10 +3619,10 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="C92" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="D92" t="s">
         <v>134</v>
@@ -3631,10 +3639,10 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="C93" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="D93" t="s">
         <v>134</v>
@@ -3651,10 +3659,10 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="C94" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="D94" t="s">
         <v>134</v>
@@ -3674,7 +3682,7 @@
         <v>264</v>
       </c>
       <c r="C95" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="D95" t="s">
         <v>135</v>
@@ -3694,7 +3702,7 @@
         <v>324</v>
       </c>
       <c r="C96" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="D96" t="s">
         <v>135</v>
@@ -3711,10 +3719,10 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="C97" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="D97" t="s">
         <v>135</v>
@@ -3734,7 +3742,7 @@
         <v>271</v>
       </c>
       <c r="C98" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="D98" t="s">
         <v>134</v>
@@ -3754,7 +3762,7 @@
         <v>274</v>
       </c>
       <c r="C99" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="D99" t="s">
         <v>134</v>
@@ -3774,7 +3782,7 @@
         <v>276</v>
       </c>
       <c r="C100" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="D100" t="s">
         <v>134</v>
@@ -3794,7 +3802,7 @@
         <v>279</v>
       </c>
       <c r="C101" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="D101" t="s">
         <v>134</v>
@@ -3814,7 +3822,7 @@
         <v>283</v>
       </c>
       <c r="C102" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="D102" t="s">
         <v>134</v>
@@ -3834,7 +3842,7 @@
         <v>286</v>
       </c>
       <c r="C103" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="D103" t="s">
         <v>134</v>
@@ -3854,7 +3862,7 @@
         <v>288</v>
       </c>
       <c r="C104" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D104" t="s">
         <v>134</v>
@@ -3874,7 +3882,7 @@
         <v>292</v>
       </c>
       <c r="C105" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="D105" t="s">
         <v>134</v>
@@ -3894,7 +3902,7 @@
         <v>293</v>
       </c>
       <c r="C106" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="D106" t="s">
         <v>135</v>
@@ -3914,7 +3922,7 @@
         <v>296</v>
       </c>
       <c r="C107" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="D107" t="s">
         <v>135</v>
@@ -3934,7 +3942,7 @@
         <v>301</v>
       </c>
       <c r="C108" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="D108" t="s">
         <v>135</v>
@@ -3954,7 +3962,7 @@
         <v>302</v>
       </c>
       <c r="C109" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="D109" t="s">
         <v>135</v>
@@ -3974,7 +3982,7 @@
         <v>305</v>
       </c>
       <c r="C110" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="D110" t="s">
         <v>135</v>
@@ -3994,7 +4002,7 @@
         <v>307</v>
       </c>
       <c r="C111" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="D111" t="s">
         <v>135</v>
@@ -4014,7 +4022,7 @@
         <v>310</v>
       </c>
       <c r="C112" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="D112" t="s">
         <v>134</v>
@@ -4034,7 +4042,7 @@
         <v>312</v>
       </c>
       <c r="C113" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="D113" t="s">
         <v>134</v>
@@ -4054,7 +4062,7 @@
         <v>316</v>
       </c>
       <c r="C114" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D114" t="s">
         <v>134</v>
@@ -4074,7 +4082,7 @@
         <v>320</v>
       </c>
       <c r="C115" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="D115" t="s">
         <v>135</v>
@@ -4094,7 +4102,7 @@
         <v>321</v>
       </c>
       <c r="C116" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="D116" t="s">
         <v>135</v>
@@ -4114,7 +4122,7 @@
         <v>206</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>134</v>
@@ -4123,7 +4131,7 @@
         <v>209</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adjust parse and getCktOrigin functions for resistors
</commit_message>
<xml_diff>
--- a/src/main/webapp/js/cktparser/drawio_circuitikz_v19082022.xlsx
+++ b/src/main/webapp/js/cktparser/drawio_circuitikz_v19082022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yuriel\git\CJ1-drawio-circuitikz\src\main\webapp\js\cktparser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE8E07E-F562-4257-9899-53576E312154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B78DFAB-9E15-4958-A7E6-152944E3CAA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{ACCEF36F-F2B4-4F7F-83FE-D2DAA1238264}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="450">
   <si>
     <t>Name</t>
   </si>
@@ -1185,12 +1185,6 @@
   </si>
   <si>
     <t>memristor</t>
-  </si>
-  <si>
-    <t>phr</t>
-  </si>
-  <si>
-    <t>pr</t>
   </si>
   <si>
     <t>capacitor</t>
@@ -1757,12 +1751,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A398772A-703D-48FD-983F-987E309B1154}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:H117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B118" sqref="B118"/>
+      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1775,7 +1770,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B1" t="s">
         <v>330</v>
@@ -1793,7 +1788,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1813,7 +1808,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1833,7 +1828,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1853,12 +1848,12 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C5" t="s">
         <v>337</v>
@@ -1873,7 +1868,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1893,7 +1888,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1913,7 +1908,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1933,7 +1928,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1953,7 +1948,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1973,7 +1968,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1993,7 +1988,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2013,7 +2008,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2033,7 +2028,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2053,7 +2048,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2073,7 +2068,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -2081,7 +2076,7 @@
         <v>30</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>135</v>
@@ -2093,7 +2088,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -2101,7 +2096,7 @@
         <v>31</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>135</v>
@@ -2164,7 +2159,7 @@
         <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>384</v>
+        <v>54</v>
       </c>
       <c r="D20" t="s">
         <v>134</v>
@@ -2187,7 +2182,7 @@
         <v>37</v>
       </c>
       <c r="C21" t="s">
-        <v>384</v>
+        <v>53</v>
       </c>
       <c r="D21" t="s">
         <v>134</v>
@@ -2299,7 +2294,7 @@
         <v>48</v>
       </c>
       <c r="C26" t="s">
-        <v>383</v>
+        <v>416</v>
       </c>
       <c r="D26" t="s">
         <v>134</v>
@@ -2322,7 +2317,7 @@
         <v>80</v>
       </c>
       <c r="C27" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D27" t="s">
         <v>134</v>
@@ -2342,7 +2337,7 @@
         <v>81</v>
       </c>
       <c r="C28" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D28" t="s">
         <v>134</v>
@@ -2362,7 +2357,7 @@
         <v>82</v>
       </c>
       <c r="C29" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D29" t="s">
         <v>134</v>
@@ -2382,7 +2377,7 @@
         <v>83</v>
       </c>
       <c r="C30" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D30" t="s">
         <v>134</v>
@@ -2402,7 +2397,7 @@
         <v>86</v>
       </c>
       <c r="C31" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D31" t="s">
         <v>134</v>
@@ -2442,7 +2437,7 @@
         <v>88</v>
       </c>
       <c r="C33" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D33" t="s">
         <v>134</v>
@@ -2462,7 +2457,7 @@
         <v>89</v>
       </c>
       <c r="C34" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="D34" t="s">
         <v>134</v>
@@ -2474,7 +2469,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2482,7 +2477,7 @@
         <v>92</v>
       </c>
       <c r="C35" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D35" t="s">
         <v>135</v>
@@ -2494,7 +2489,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2502,7 +2497,7 @@
         <v>94</v>
       </c>
       <c r="C36" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="D36" t="s">
         <v>135</v>
@@ -2514,7 +2509,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2562,7 +2557,7 @@
         <v>108</v>
       </c>
       <c r="C39" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D39" t="s">
         <v>134</v>
@@ -2582,7 +2577,7 @@
         <v>118</v>
       </c>
       <c r="C40" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D40" t="s">
         <v>134</v>
@@ -2602,7 +2597,7 @@
         <v>119</v>
       </c>
       <c r="C41" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D41" t="s">
         <v>134</v>
@@ -2622,7 +2617,7 @@
         <v>120</v>
       </c>
       <c r="C42" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D42" t="s">
         <v>134</v>
@@ -2642,7 +2637,7 @@
         <v>121</v>
       </c>
       <c r="C43" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D43" t="s">
         <v>134</v>
@@ -2662,7 +2657,7 @@
         <v>122</v>
       </c>
       <c r="C44" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D44" t="s">
         <v>134</v>
@@ -2682,7 +2677,7 @@
         <v>123</v>
       </c>
       <c r="C45" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D45" t="s">
         <v>134</v>
@@ -2702,7 +2697,7 @@
         <v>124</v>
       </c>
       <c r="C46" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D46" t="s">
         <v>134</v>
@@ -2722,7 +2717,7 @@
         <v>125</v>
       </c>
       <c r="C47" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D47" t="s">
         <v>134</v>
@@ -2742,7 +2737,7 @@
         <v>142</v>
       </c>
       <c r="C48" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D48" t="s">
         <v>134</v>
@@ -2762,7 +2757,7 @@
         <v>145</v>
       </c>
       <c r="C49" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D49" t="s">
         <v>134</v>
@@ -2782,7 +2777,7 @@
         <v>149</v>
       </c>
       <c r="C50" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D50" t="s">
         <v>134</v>
@@ -2802,7 +2797,7 @@
         <v>148</v>
       </c>
       <c r="C51" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D51" t="s">
         <v>134</v>
@@ -2822,7 +2817,7 @@
         <v>150</v>
       </c>
       <c r="C52" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D52" t="s">
         <v>134</v>
@@ -2839,10 +2834,10 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C53" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D53" t="s">
         <v>134</v>
@@ -2862,7 +2857,7 @@
         <v>153</v>
       </c>
       <c r="C54" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D54" t="s">
         <v>134</v>
@@ -2882,7 +2877,7 @@
         <v>109</v>
       </c>
       <c r="C55" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D55" t="s">
         <v>134</v>
@@ -2902,7 +2897,7 @@
         <v>146</v>
       </c>
       <c r="C56" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D56" t="s">
         <v>134</v>
@@ -2922,7 +2917,7 @@
         <v>147</v>
       </c>
       <c r="C57" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D57" t="s">
         <v>134</v>
@@ -2942,7 +2937,7 @@
         <v>152</v>
       </c>
       <c r="C58" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D58" t="s">
         <v>134</v>
@@ -2962,7 +2957,7 @@
         <v>151</v>
       </c>
       <c r="C59" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D59" t="s">
         <v>134</v>
@@ -2974,7 +2969,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2994,7 +2989,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>60</v>
       </c>
@@ -3014,7 +3009,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>61</v>
       </c>
@@ -3034,7 +3029,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>62</v>
       </c>
@@ -3054,7 +3049,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>63</v>
       </c>
@@ -3074,7 +3069,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>64</v>
       </c>
@@ -3094,7 +3089,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>65</v>
       </c>
@@ -3114,7 +3109,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>66</v>
       </c>
@@ -3134,7 +3129,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>67</v>
       </c>
@@ -3154,7 +3149,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>68</v>
       </c>
@@ -3174,7 +3169,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>69</v>
       </c>
@@ -3194,7 +3189,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>70</v>
       </c>
@@ -3214,7 +3209,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>71</v>
       </c>
@@ -3234,7 +3229,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>72</v>
       </c>
@@ -3259,10 +3254,10 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C74" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D74" t="s">
         <v>134</v>
@@ -3282,7 +3277,7 @@
         <v>205</v>
       </c>
       <c r="C75" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D75" t="s">
         <v>134</v>
@@ -3299,10 +3294,10 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C76" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D76" t="s">
         <v>134</v>
@@ -3322,7 +3317,7 @@
         <v>217</v>
       </c>
       <c r="C77" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D77" t="s">
         <v>134</v>
@@ -3342,7 +3337,7 @@
         <v>220</v>
       </c>
       <c r="C78" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D78" t="s">
         <v>134</v>
@@ -3362,7 +3357,7 @@
         <v>222</v>
       </c>
       <c r="C79" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D79" t="s">
         <v>134</v>
@@ -3374,7 +3369,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>79</v>
       </c>
@@ -3394,7 +3389,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>80</v>
       </c>
@@ -3422,7 +3417,7 @@
         <v>231</v>
       </c>
       <c r="C82" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D82" t="s">
         <v>134</v>
@@ -3442,7 +3437,7 @@
         <v>232</v>
       </c>
       <c r="C83" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D83" t="s">
         <v>134</v>
@@ -3462,7 +3457,7 @@
         <v>233</v>
       </c>
       <c r="C84" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D84" t="s">
         <v>134</v>
@@ -3482,7 +3477,7 @@
         <v>234</v>
       </c>
       <c r="C85" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D85" t="s">
         <v>134</v>
@@ -3494,7 +3489,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>85</v>
       </c>
@@ -3514,7 +3509,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>86</v>
       </c>
@@ -3534,7 +3529,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>87</v>
       </c>
@@ -3554,7 +3549,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>88</v>
       </c>
@@ -3574,7 +3569,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>89</v>
       </c>
@@ -3599,10 +3594,10 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C91" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D91" t="s">
         <v>134</v>
@@ -3619,10 +3614,10 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C92" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D92" t="s">
         <v>134</v>
@@ -3639,10 +3634,10 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C93" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D93" t="s">
         <v>134</v>
@@ -3659,10 +3654,10 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C94" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D94" t="s">
         <v>134</v>
@@ -3674,7 +3669,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>94</v>
       </c>
@@ -3694,7 +3689,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>95</v>
       </c>
@@ -3714,12 +3709,12 @@
         <v>266</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C97" t="s">
         <v>370</v>
@@ -3742,7 +3737,7 @@
         <v>271</v>
       </c>
       <c r="C98" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D98" t="s">
         <v>134</v>
@@ -3762,7 +3757,7 @@
         <v>274</v>
       </c>
       <c r="C99" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D99" t="s">
         <v>134</v>
@@ -3782,7 +3777,7 @@
         <v>276</v>
       </c>
       <c r="C100" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="D100" t="s">
         <v>134</v>
@@ -3802,7 +3797,7 @@
         <v>279</v>
       </c>
       <c r="C101" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="D101" t="s">
         <v>134</v>
@@ -3822,7 +3817,7 @@
         <v>283</v>
       </c>
       <c r="C102" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="D102" t="s">
         <v>134</v>
@@ -3842,7 +3837,7 @@
         <v>286</v>
       </c>
       <c r="C103" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="D103" t="s">
         <v>134</v>
@@ -3862,7 +3857,7 @@
         <v>288</v>
       </c>
       <c r="C104" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D104" t="s">
         <v>134</v>
@@ -3882,7 +3877,7 @@
         <v>292</v>
       </c>
       <c r="C105" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="D105" t="s">
         <v>134</v>
@@ -3894,7 +3889,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>105</v>
       </c>
@@ -3914,7 +3909,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>106</v>
       </c>
@@ -3934,7 +3929,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>107</v>
       </c>
@@ -3954,7 +3949,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>108</v>
       </c>
@@ -3974,7 +3969,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>109</v>
       </c>
@@ -3994,7 +3989,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>110</v>
       </c>
@@ -4022,7 +4017,7 @@
         <v>310</v>
       </c>
       <c r="C112" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D112" t="s">
         <v>134</v>
@@ -4042,7 +4037,7 @@
         <v>312</v>
       </c>
       <c r="C113" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="D113" t="s">
         <v>134</v>
@@ -4062,7 +4057,7 @@
         <v>316</v>
       </c>
       <c r="C114" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="D114" t="s">
         <v>134</v>
@@ -4074,7 +4069,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>114</v>
       </c>
@@ -4094,7 +4089,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>115</v>
       </c>
@@ -4122,7 +4117,7 @@
         <v>206</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>134</v>
@@ -4131,11 +4126,20 @@
         <v>209</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F117" xr:uid="{A398772A-703D-48FD-983F-987E309B1154}"/>
+  <autoFilter ref="A1:F117" xr:uid="{A398772A-703D-48FD-983F-987E309B1154}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="path"/>
+      </filters>
+    </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A18:F117">
+      <sortCondition ref="A1:A117"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>